<commit_message>
added weapon sockets option, changed to dictionary
</commit_message>
<xml_diff>
--- a/Assets/Resources/ItemData/Randomize/WeaponRadomizeByLevel.xlsx
+++ b/Assets/Resources/ItemData/Randomize/WeaponRadomizeByLevel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PSG\Desktop\Capstone-Design-Project\Assets\Resources\ItemData\Randomize\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A620DF-D818-4CAE-BD57-86965176E112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F085714-F77E-407C-AEFD-CD19A08E5719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2892" yWindow="720" windowWidth="19332" windowHeight="11172" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,13 +25,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>ATK</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ATKSPEED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOCKET</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -357,92 +361,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>5</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>7</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>9</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>11</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>13</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>15</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>17</v>
       </c>
       <c r="B10">
         <v>9</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>